<commit_message>
Proyecto de Gestor de Empresas
</commit_message>
<xml_diff>
--- a/Business Manager/companies.xlsx
+++ b/Business Manager/companies.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Company Name</t>
   </si>
@@ -49,13 +49,16 @@
     <t>Medium</t>
   </si>
   <si>
-    <t>Dennys</t>
+    <t>Trivago</t>
   </si>
   <si>
     <t>10</t>
   </si>
   <si>
     <t>Low</t>
+  </si>
+  <si>
+    <t>"65e4a51476cc4294f12ba119"</t>
   </si>
 </sst>
 </file>
@@ -508,7 +511,7 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>